<commit_message>
Fix resourceType inference on the StructureMap tool
</commit_message>
<xml_diff>
--- a/structure-map-tool/src/main/resources/StructureMap XLS.xlsx
+++ b/structure-map-tool/src/main/resources/StructureMap XLS.xlsx
@@ -215,7 +215,7 @@
     <t xml:space="preserve">???</t>
   </si>
   <si>
-    <t xml:space="preserve">RiskFlag</t>
+    <t xml:space="preserve">Flag</t>
   </si>
   <si>
     <t xml:space="preserve">http://hl7.org/fhir/StructureDefinition/flag-detail</t>
@@ -501,11 +501,11 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
@@ -1011,8 +1011,8 @@
     <hyperlink ref="B38" r:id="rId5" display="http://hl7.org/fhir/StructureDefinition/flag-detail"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1031,7 +1031,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.5"/>
@@ -1085,8 +1085,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fix bugs and add TODOs
- Update remaining TODO tasks and comments
- Add resource extraction for testing
- Add RiskAssessmentPrediction entity create support with reflection class name
- Fix group names
- Fix datatype of constant value mapping
- Fix dollar sign escaping when mapping QR values to resource elements
- Fix bug with empty conversion values
</commit_message>
<xml_diff>
--- a/structure-map-tool/src/main/resources/StructureMap XLS.xlsx
+++ b/structure-map-tool/src/main/resources/StructureMap XLS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t xml:space="preserve">Questionnaire Response Field Id</t>
   </si>
@@ -62,9 +62,6 @@
     <t xml:space="preserve">name.family</t>
   </si>
   <si>
-    <t xml:space="preserve">field * 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">PR-name-given</t>
   </si>
   <si>
@@ -158,7 +155,7 @@
     <t xml:space="preserve">effective</t>
   </si>
   <si>
-    <t xml:space="preserve">evaluate(Patient, now())</t>
+    <t xml:space="preserve">evaluate(src, now())</t>
   </si>
   <si>
     <t xml:space="preserve">code</t>
@@ -502,10 +499,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
@@ -579,63 +576,61 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,71 +641,71 @@
         <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -718,46 +713,46 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,229 +760,229 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="H22" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1031,7 +1026,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.5"/>
@@ -1040,14 +1035,14 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1074,13 +1069,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>